<commit_message>
se hace mas rapido
</commit_message>
<xml_diff>
--- a/saves/Lentejas y cosas_full.xlsx
+++ b/saves/Lentejas y cosas_full.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -1251,10 +1251,19 @@
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1265,15 +1274,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1581,10 +1581,10 @@
   <dimension ref="A1:FT17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="J3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="2" topLeftCell="Q3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="T2" sqref="T2"/>
+      <selection pane="bottomRight" activeCell="AA2" sqref="AA2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1597,7 +1597,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:176" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="14"/>
@@ -1605,7 +1605,7 @@
       <c r="D1" s="14"/>
       <c r="E1" s="14"/>
       <c r="F1" s="14"/>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="18" t="s">
         <v>1</v>
       </c>
       <c r="H1" s="14"/>
@@ -1617,7 +1617,7 @@
       <c r="N1" s="14"/>
       <c r="O1" s="14"/>
       <c r="P1" s="14"/>
-      <c r="Q1" s="21" t="s">
+      <c r="Q1" s="16" t="s">
         <v>2</v>
       </c>
       <c r="R1" s="14"/>
@@ -1632,7 +1632,7 @@
       <c r="AA1" s="14"/>
       <c r="AB1" s="14"/>
       <c r="AC1" s="14"/>
-      <c r="AD1" s="17" t="s">
+      <c r="AD1" s="20" t="s">
         <v>3</v>
       </c>
       <c r="AE1" s="14"/>
@@ -1646,7 +1646,7 @@
       <c r="AM1" s="14"/>
       <c r="AN1" s="14"/>
       <c r="AO1" s="14"/>
-      <c r="AP1" s="13" t="s">
+      <c r="AP1" s="17" t="s">
         <v>4</v>
       </c>
       <c r="AQ1" s="14"/>
@@ -1700,7 +1700,7 @@
       <c r="CM1" s="14"/>
       <c r="CN1" s="14"/>
       <c r="CO1" s="14"/>
-      <c r="CP1" s="16" t="s">
+      <c r="CP1" s="19" t="s">
         <v>5</v>
       </c>
       <c r="CQ1" s="14"/>
@@ -1754,7 +1754,7 @@
       <c r="EM1" s="14"/>
       <c r="EN1" s="14"/>
       <c r="EO1" s="14"/>
-      <c r="EP1" s="20" t="s">
+      <c r="EP1" s="15" t="s">
         <v>6</v>
       </c>
       <c r="EQ1" s="14"/>
@@ -1779,7 +1779,7 @@
       <c r="FJ1" s="14"/>
       <c r="FK1" s="14"/>
       <c r="FL1" s="14"/>
-      <c r="FM1" s="19" t="s">
+      <c r="FM1" s="13" t="s">
         <v>7</v>
       </c>
       <c r="FN1" s="14"/>
@@ -4816,6 +4816,7 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A1:F1"/>
     <mergeCell ref="FM1:FT1"/>
     <mergeCell ref="EP1:FL1"/>
     <mergeCell ref="Q1:AC1"/>
@@ -4823,7 +4824,6 @@
     <mergeCell ref="G1:P1"/>
     <mergeCell ref="CP1:EO1"/>
     <mergeCell ref="AD1:AO1"/>
-    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>